<commit_message>
Added readme for the file descriptions
</commit_message>
<xml_diff>
--- a/src/pdl/Files.xlsx
+++ b/src/pdl/Files.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Masters\dissertation\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Masters\dissertation_code\src\pdl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6BB501-0B9F-4115-832A-29393A9DBF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8A2A32-76E2-4AE5-B865-B0D3041B42BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,9 +78,6 @@
     <t>Solution 5</t>
   </si>
   <si>
-    <t xml:space="preserve">Used for qualitative evaluation of Approach 2 on both original and retrained models many different datasets. </t>
-  </si>
-  <si>
     <t>Used for quantitative testing for Approach 2 on solution 2 converted validation set</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>Baseline - Panoptic Segmentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used for qualitative evaluation of Approach 2 on both original and retrained models for different datasets. </t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,31 +533,31 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -569,7 +569,7 @@
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
@@ -581,7 +581,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
@@ -609,7 +609,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>11</v>
@@ -623,7 +623,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>11</v>
@@ -637,7 +637,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>11</v>
@@ -651,10 +651,10 @@
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>9</v>
@@ -665,10 +665,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>9</v>

</xml_diff>